<commit_message>
separate packages for payments
</commit_message>
<xml_diff>
--- a/proVidioETG/testDate/Simple Products Skew.xlsx
+++ b/proVidioETG/testDate/Simple Products Skew.xlsx
@@ -20,12 +20,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t xml:space="preserve">Simple product</t>
   </si>
   <si>
-    <t xml:space="preserve">793775064963M</t>
+    <t xml:space="preserve">013742002836M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">013742003321M</t>
   </si>
 </sst>
 </file>
@@ -35,7 +38,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -56,11 +59,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -114,7 +112,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -135,10 +133,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -158,6 +156,11 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>